<commit_message>
minor updates to file
</commit_message>
<xml_diff>
--- a/excel_files/cement_inventory.xlsx
+++ b/excel_files/cement_inventory.xlsx
@@ -1036,7 +1036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="3" t="s">
         <v>37</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="3" t="s">
         <v>34</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="3" t="s">
         <v>49</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="3" t="s">
         <v>49</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="3" t="s">
         <v>49</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="3" t="s">
         <v>49</v>
       </c>

</xml_diff>